<commit_message>
Update LDF Survival Model Example.xlsx
</commit_message>
<xml_diff>
--- a/LDF Survival Model Example.xlsx
+++ b/LDF Survival Model Example.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiigroup-my.sharepoint.com/personal/ukorn_skywardinsurance_com/Documents/Documents/paps/Survival LDFs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1477" documentId="8_{CC31E55A-8BBB-40EB-81A7-0EE13C01BAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77DC041E-0865-48E1-9BDE-4EC63CB655F1}"/>
+  <xr:revisionPtr revIDLastSave="1611" documentId="8_{CC31E55A-8BBB-40EB-81A7-0EE13C01BAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEDC85C2-50E3-4902-B48E-ED68807D00C5}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="400" windowWidth="15830" windowHeight="10140" xr2:uid="{B66CFAF0-0D28-4DA0-AD47-F99DD1328259}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{B66CFAF0-0D28-4DA0-AD47-F99DD1328259}"/>
   </bookViews>
   <sheets>
-    <sheet name="Example 1" sheetId="3" r:id="rId1"/>
-    <sheet name="Example 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Example 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Example 2" sheetId="3" r:id="rId2"/>
     <sheet name="splines" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -460,28 +460,28 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.9029239073293893</c:v>
+                  <c:v>1.2120785266443335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7176403578039845</c:v>
+                  <c:v>1.1747156978068798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2035980884610018</c:v>
+                  <c:v>1.0614058863924769</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.176660464056507</c:v>
+                  <c:v>1.0524413548375706</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2612344230749442</c:v>
+                  <c:v>1.0619182485971845</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95069520159160137</c:v>
+                  <c:v>0.99924033436634618</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1793271201979112</c:v>
+                  <c:v>1.0690214909014535</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0084787350054525</c:v>
+                  <c:v>0.9777246598710464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -489,7 +489,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-07D9-49EE-A3C0-C21B264BF5B8}"/>
+              <c16:uniqueId val="{00000000-729F-4850-BCF8-45433BF59F14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -510,7 +510,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -577,28 +577,28 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.8691822523168107</c:v>
+                  <c:v>1.2453194406796648</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5177884080037989</c:v>
+                  <c:v>1.1338511675761382</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3357741135348276</c:v>
+                  <c:v>1.0853228390154808</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.22380451183723</c:v>
+                  <c:v>1.0578045795655597</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1471070668184284</c:v>
+                  <c:v>1.0399276241393027</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0907301438535801</c:v>
+                  <c:v>1.0273052593267167</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.047196757476496</c:v>
+                  <c:v>1.0178762760567481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0123426128549904</c:v>
+                  <c:v>1.0105404238200517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,7 +606,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-07D9-49EE-A3C0-C21B264BF5B8}"/>
+              <c16:uniqueId val="{00000001-729F-4850-BCF8-45433BF59F14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -694,28 +694,28 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.1500017235279847</c:v>
+                  <c:v>1.3277944957769152</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1896296885437576</c:v>
+                  <c:v>1.0623756487948866</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0527845053155145</c:v>
+                  <c:v>1.0192198839223674</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0195751384879448</c:v>
+                  <c:v>1.0077122899381779</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0087039080882505</c:v>
+                  <c:v>1.0036573302629095</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0043864231943886</c:v>
+                  <c:v>1.001946300418612</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0024227824571046</c:v>
+                  <c:v>1.0011269375866538</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0014352320923703</c:v>
+                  <c:v>1.0006959492942842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,7 +723,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-07D9-49EE-A3C0-C21B264BF5B8}"/>
+              <c16:uniqueId val="{00000002-729F-4850-BCF8-45433BF59F14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1029,31 +1029,31 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.4271249164767763</c:v>
+                  <c:v>1.8357976563638536</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9029239073293893</c:v>
+                  <c:v>1.2120785266443335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7176403578039845</c:v>
+                  <c:v>1.1747156978068798</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2035980884610018</c:v>
+                  <c:v>1.0614058863924769</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.176660464056507</c:v>
+                  <c:v>1.0524413548375706</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2612344230749442</c:v>
+                  <c:v>1.0619182485971845</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.95069520159160137</c:v>
+                  <c:v>0.99924033436634618</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1793271201979112</c:v>
+                  <c:v>1.0690214909014535</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0084787350054525</c:v>
+                  <c:v>0.9777246598710464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,7 +1061,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-45FE-4B14-A4F4-9C7C037E4B35}"/>
+              <c16:uniqueId val="{00000000-02A0-485A-BDE8-8988678A3099}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1082,7 +1082,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1152,31 +1152,31 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.5888285219745275</c:v>
+                  <c:v>1.8174446792532741</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8691822523168107</c:v>
+                  <c:v>1.2453194406796648</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5177884080037989</c:v>
+                  <c:v>1.1338511675761382</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3357741135348276</c:v>
+                  <c:v>1.0853228390154808</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.22380451183723</c:v>
+                  <c:v>1.0578045795655597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1471070668184284</c:v>
+                  <c:v>1.0399276241393027</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0907301438535801</c:v>
+                  <c:v>1.0273052593267167</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.047196757476496</c:v>
+                  <c:v>1.0178762760567481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0123426128549904</c:v>
+                  <c:v>1.0105404238200517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1184,7 +1184,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-45FE-4B14-A4F4-9C7C037E4B35}"/>
+              <c16:uniqueId val="{00000001-02A0-485A-BDE8-8988678A3099}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1482,33 +1482,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Example 2'!$C$20:$J$20</c:f>
+              <c:f>'Example 2'!$C$20:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.2120785266443335</c:v>
+                  <c:v>2.349269578480516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1747156978068798</c:v>
+                  <c:v>1.4701832659905301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0614058863924769</c:v>
+                  <c:v>1.0518281414534474</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0524413548375706</c:v>
+                  <c:v>1.5341890217974079</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0619182485971845</c:v>
+                  <c:v>1.1254391168656985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94389870421798472</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0690214909014535</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.9777246598710464</c:v>
+                  <c:v>1.2162325748548299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1516,7 +1510,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-729F-4850-BCF8-45433BF59F14}"/>
+              <c16:uniqueId val="{00000000-07D9-49EE-A3C0-C21B264BF5B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1537,7 +1531,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1599,33 +1593,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Example 2'!$C$54:$J$54</c:f>
+              <c:f>'Example 2'!$C$54:$I$54</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.2440255816659809</c:v>
+                  <c:v>1.8371865633164386</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1294192410672006</c:v>
+                  <c:v>1.5128723571281022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0790691376525661</c:v>
+                  <c:v>1.3538957236352975</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0502885158504212</c:v>
+                  <c:v>1.2571792539358313</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0314557926985988</c:v>
+                  <c:v>1.1909962738973967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0180698476339016</c:v>
+                  <c:v>1.1422480792447984</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0080083432212172</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0001346832030382</c:v>
+                  <c:v>1.1044912361659469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,7 +1624,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-729F-4850-BCF8-45433BF59F14}"/>
+              <c16:uniqueId val="{00000001-07D9-49EE-A3C0-C21B264BF5B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1716,33 +1707,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Example 2'!$C$62:$J$62</c:f>
+              <c:f>'Example 2'!$C$62:$I$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.3277944957769152</c:v>
+                  <c:v>2.0934852752883728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0623756487948866</c:v>
+                  <c:v>1.1624086176775601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0192198839223674</c:v>
+                  <c:v>1.0419748422917501</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0077122899381779</c:v>
+                  <c:v>1.0146958798674344</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0036573302629095</c:v>
+                  <c:v>1.0062342642081201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.001946300418612</c:v>
+                  <c:v>1.0030193725744088</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0011269375866538</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0006959492942842</c:v>
+                  <c:v>1.0016112584460295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1750,7 +1738,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-729F-4850-BCF8-45433BF59F14}"/>
+              <c16:uniqueId val="{00000002-07D9-49EE-A3C0-C21B264BF5B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2051,36 +2039,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Example 2'!$B$20:$J$20</c:f>
+              <c:f>'Example 2'!$B$20:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.8357976563638536</c:v>
+                  <c:v>2.4271249164767763</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2120785266443335</c:v>
+                  <c:v>2.349269578480516</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1747156978068798</c:v>
+                  <c:v>1.4701832659905301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0614058863924769</c:v>
+                  <c:v>1.0518281414534474</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0524413548375706</c:v>
+                  <c:v>1.5341890217974079</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0619182485971845</c:v>
+                  <c:v>1.1254391168656985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94389870421798472</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0690214909014535</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9777246598710464</c:v>
+                  <c:v>1.2162325748548299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2088,7 +2070,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-02A0-485A-BDE8-8988678A3099}"/>
+              <c16:uniqueId val="{00000000-45FE-4B14-A4F4-9C7C037E4B35}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2109,7 +2091,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2179,31 +2161,31 @@
                 <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.8258459273790315</c:v>
+                  <c:v>2.9207320708831213</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2440255816659809</c:v>
+                  <c:v>1.8371865633164386</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1294192410672006</c:v>
+                  <c:v>1.5128723571281022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0790691376525661</c:v>
+                  <c:v>1.3538957236352975</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0502885158504212</c:v>
+                  <c:v>1.2571792539358313</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0314557926985988</c:v>
+                  <c:v>1.1909962738973967</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0180698476339016</c:v>
+                  <c:v>1.1422480792447984</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0080083432212172</c:v>
+                  <c:v>1.1044912361659469</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0001346832030382</c:v>
+                  <c:v>1.0741628334261819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2211,7 +2193,79 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-02A0-485A-BDE8-8988678A3099}"/>
+              <c16:uniqueId val="{00000001-45FE-4B14-A4F4-9C7C037E4B35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Example 2'!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inverse Power Curve</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Example 2'!$B$62:$K$62</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>29.486349965572114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0934852752883728</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1624086176775601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0419748422917501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0146958798674344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0062342642081201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0030193725744088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0016112584460295</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0009259367777132</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0005641202983839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E3A-48E8-A35D-079FD2DB7985}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2282,6 +2336,7 @@
         <c:axId val="326962448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4662,7 +4717,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC07FF7-0C0B-4284-B526-B450910385CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A97A711-DD3F-40F1-9BB0-52824F87C549}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4697,10 +4752,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5FF7E82-C87E-4318-9EB0-AF4EBBEA3705}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77D6E1D6-BB93-49CA-AFEC-4D7848BE01D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4743,7 +4798,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A97A711-DD3F-40F1-9BB0-52824F87C549}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC07FF7-0C0B-4284-B526-B450910385CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4778,10 +4833,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77D6E1D6-BB93-49CA-AFEC-4D7848BE01D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5FF7E82-C87E-4318-9EB0-AF4EBBEA3705}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5124,22 +5179,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E14914A-8E2A-4748-9C7B-BA3BA6166CC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6AC979-46A0-45AC-AD4D-731805EBF10B}">
   <dimension ref="A1:AB62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.7265625" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -5238,217 +5291,397 @@
       <c r="A4" s="2">
         <v>2013</v>
       </c>
+      <c r="B4" s="13">
+        <v>387026.80900000001</v>
+      </c>
+      <c r="C4" s="13">
+        <v>463552.06300000002</v>
+      </c>
+      <c r="D4" s="13">
+        <v>485844.29399999999</v>
+      </c>
+      <c r="E4" s="13">
+        <v>778173.73400000005</v>
+      </c>
+      <c r="F4" s="13">
+        <v>909494.57299999997</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1026309.7130000002</v>
+      </c>
+      <c r="H4" s="13">
+        <v>990261.68800000008</v>
+      </c>
+      <c r="I4" s="13">
+        <v>990261.68800000008</v>
+      </c>
+      <c r="J4" s="13">
+        <v>1025162.2289999999</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1025162.2289999999</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1025162.2289999999</v>
+      </c>
+      <c r="M4" s="13">
+        <v>1025162.2289999999</v>
+      </c>
+      <c r="N4" s="13">
+        <v>1025162.2289999999</v>
+      </c>
+      <c r="O4" s="13">
+        <v>1025162.2289999999</v>
+      </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2014</v>
       </c>
+      <c r="B5" s="13">
+        <v>721554.38100000017</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1017504.4859999997</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1986074.2079999994</v>
+      </c>
+      <c r="E5" s="13">
+        <v>2575477.6020000004</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3477456.1260000006</v>
+      </c>
+      <c r="G5" s="13">
+        <v>3247546.0949999993</v>
+      </c>
+      <c r="H5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="I5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="J5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="K5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="L5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="M5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="N5" s="13">
+        <v>3246444.3689999995</v>
+      </c>
+      <c r="O5" s="13"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2015</v>
       </c>
+      <c r="B6" s="13">
+        <v>3512563.7219999991</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5266562.3999999976</v>
+      </c>
+      <c r="D6" s="13">
+        <v>6351170.7869999949</v>
+      </c>
+      <c r="E6" s="13">
+        <v>7008749.8739999942</v>
+      </c>
+      <c r="F6" s="13">
+        <v>7839785.8529999955</v>
+      </c>
+      <c r="G6" s="13">
+        <v>7643692.7009999957</v>
+      </c>
+      <c r="H6" s="13">
+        <v>7600920.3179999935</v>
+      </c>
+      <c r="I6" s="13">
+        <v>7601336.3969999934</v>
+      </c>
+      <c r="J6" s="13">
+        <v>8654880</v>
+      </c>
+      <c r="K6" s="13">
+        <v>7600713.1379999937</v>
+      </c>
+      <c r="L6" s="13">
+        <v>7600713.1379999937</v>
+      </c>
+      <c r="M6" s="13">
+        <v>7600713.1379999937</v>
+      </c>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2016</v>
       </c>
+      <c r="B7" s="13">
+        <v>4870653.2379999934</v>
+      </c>
+      <c r="C7" s="13">
+        <v>8588861.5669999961</v>
+      </c>
+      <c r="D7" s="13">
+        <v>14932191.723000005</v>
+      </c>
+      <c r="E7" s="13">
+        <v>17189503.470999993</v>
+      </c>
+      <c r="F7" s="13">
+        <v>17301048.222999994</v>
+      </c>
+      <c r="G7" s="13">
+        <v>17271026.528999999</v>
+      </c>
+      <c r="H7" s="13">
+        <v>17271833.025999997</v>
+      </c>
+      <c r="I7" s="13">
+        <v>17266960.128999997</v>
+      </c>
+      <c r="J7" s="13">
+        <v>17267699.628999997</v>
+      </c>
+      <c r="K7" s="13">
+        <v>17267699.628999997</v>
+      </c>
+      <c r="L7" s="13">
+        <v>17267699.628999997</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2017</v>
       </c>
       <c r="B8" s="13">
-        <v>7719</v>
+        <v>5768068.1924999971</v>
       </c>
       <c r="C8" s="13">
-        <v>17079</v>
+        <v>10037063.895000013</v>
       </c>
       <c r="D8" s="13">
-        <v>32138</v>
+        <v>10652257.732500013</v>
       </c>
       <c r="E8" s="13">
-        <v>55930</v>
+        <v>12006271.860000012</v>
       </c>
       <c r="F8" s="13">
-        <v>75400</v>
+        <v>12089139.85500001</v>
       </c>
       <c r="G8" s="13">
-        <v>99711</v>
+        <v>12769212.660000011</v>
       </c>
       <c r="H8" s="13">
-        <v>113647</v>
+        <v>14135430.285000011</v>
       </c>
       <c r="I8" s="13">
-        <v>104617</v>
+        <v>14025377.182500012</v>
       </c>
       <c r="J8" s="13">
-        <v>110040</v>
+        <v>14942623.410000008</v>
       </c>
       <c r="K8" s="13">
-        <v>110973</v>
-      </c>
+        <v>14991352.485000009</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2018</v>
       </c>
       <c r="B9" s="13">
-        <v>6387</v>
+        <v>5019038.7225000057</v>
       </c>
       <c r="C9" s="13">
-        <v>17842</v>
+        <v>7594422.4050000068</v>
       </c>
       <c r="D9" s="13">
-        <v>35429</v>
+        <v>8270724.5700000059</v>
       </c>
       <c r="E9" s="13">
-        <v>57222</v>
+        <v>8827020.8699999973</v>
       </c>
       <c r="F9" s="13">
-        <v>80791</v>
+        <v>9476244.7874999959</v>
       </c>
       <c r="G9" s="13">
-        <v>95150</v>
+        <v>9398204.8799999971</v>
       </c>
       <c r="H9" s="13">
-        <v>120432</v>
+        <v>9247393.0574999955</v>
       </c>
       <c r="I9" s="13">
-        <v>112450</v>
+        <v>9630246.577499995</v>
       </c>
       <c r="J9" s="13">
-        <v>145953</v>
+        <v>11231985</v>
       </c>
       <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>2019</v>
       </c>
       <c r="B10" s="13">
-        <v>8347</v>
+        <v>4799936.1359999962</v>
       </c>
       <c r="C10" s="13">
-        <v>18022</v>
+        <v>9923861.3215200026</v>
       </c>
       <c r="D10" s="13">
-        <v>36758</v>
+        <v>11191566.177540002</v>
       </c>
       <c r="E10" s="13">
-        <v>71537</v>
+        <v>11744990.166240001</v>
       </c>
       <c r="F10" s="13">
-        <v>87621</v>
+        <v>11492856.698519999</v>
       </c>
       <c r="G10" s="13">
-        <v>100813</v>
+        <v>13545433</v>
       </c>
       <c r="H10" s="13">
-        <v>121789</v>
+        <v>16304933</v>
       </c>
       <c r="I10" s="13">
-        <v>121255</v>
+        <v>15987545</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2020</v>
       </c>
       <c r="B11" s="13">
-        <v>7700</v>
+        <v>5493944.7647999981</v>
       </c>
       <c r="C11" s="13">
-        <v>21502</v>
+        <v>9782584.9694000017</v>
       </c>
       <c r="D11" s="13">
-        <v>43272</v>
+        <v>11469778.782000007</v>
       </c>
       <c r="E11" s="13">
-        <v>64383</v>
+        <v>13748603.980399996</v>
       </c>
       <c r="F11" s="13">
-        <v>78572</v>
+        <v>15373592.092799991</v>
       </c>
       <c r="G11" s="13">
-        <v>93042</v>
+        <v>15553060.047999991</v>
       </c>
       <c r="H11" s="13">
-        <v>134394</v>
+        <v>15821034.859000001</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>2021</v>
       </c>
       <c r="B12" s="13">
-        <v>8223</v>
+        <v>3957732.8453999995</v>
       </c>
       <c r="C12" s="13">
-        <v>23181</v>
+        <v>7073422.3987300014</v>
       </c>
       <c r="D12" s="13">
-        <v>37376</v>
+        <v>9012357.8970860001</v>
       </c>
       <c r="E12" s="13">
-        <v>67965</v>
+        <v>12220604.864725998</v>
       </c>
       <c r="F12" s="13">
-        <v>72611</v>
+        <v>12527619.908443999</v>
       </c>
       <c r="G12" s="13">
-        <v>76059</v>
+        <v>12890339.077689998</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>2022</v>
       </c>
       <c r="B13" s="13">
-        <v>12122</v>
+        <v>4420890.5543999989</v>
       </c>
       <c r="C13" s="13">
-        <v>26156</v>
+        <v>6193275.3660000023</v>
       </c>
       <c r="D13" s="13">
-        <v>48834</v>
+        <v>8009139.5616000025</v>
       </c>
       <c r="E13" s="13">
-        <v>82909</v>
+        <v>8449642.2374880016</v>
       </c>
       <c r="F13" s="13">
-        <v>94462</v>
+        <v>9497311.2634847071</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2023</v>
       </c>
       <c r="B14" s="13">
-        <v>7596</v>
+        <v>3503613.7829999998</v>
       </c>
       <c r="C14" s="13">
-        <v>19404</v>
+        <v>6135103.6164999977</v>
       </c>
       <c r="D14" s="13">
-        <v>65507</v>
+        <v>6985432.0978999939</v>
       </c>
       <c r="E14" s="13">
-        <v>111264</v>
+        <v>8658113.4147999957</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -5456,19 +5689,23 @@
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2024</v>
       </c>
       <c r="B15" s="13">
-        <v>10264</v>
+        <v>7754842.6332499953</v>
       </c>
       <c r="C15" s="13">
-        <v>44816</v>
+        <v>13049523.252849992</v>
       </c>
       <c r="D15" s="13">
-        <v>62018</v>
+        <v>15714106.588029997</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -5477,16 +5714,20 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2025</v>
       </c>
       <c r="B16" s="13">
-        <v>20162</v>
+        <v>5291461.7594000008</v>
       </c>
       <c r="C16" s="13">
-        <v>28107</v>
+        <v>13312433.566699998</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -5496,13 +5737,17 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>2026</v>
       </c>
       <c r="B17" s="13">
-        <v>10682</v>
+        <v>6373903.717600002</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -5513,9 +5758,22 @@
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
@@ -5573,50 +5831,54 @@
       </c>
       <c r="B20" s="4">
         <f ca="1">SUM(OFFSET(C13:C17,-B19-1,0))/SUM(OFFSET(B13:B17,-B19-1,0))</f>
-        <v>2.4271249164767763</v>
+        <v>1.8357976563638536</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" ref="C20:J20" ca="1" si="0">SUM(OFFSET(D13:D17,-C19-1,0))/SUM(OFFSET(C13:C17,-C19-1,0))</f>
-        <v>1.9029239073293893</v>
+        <v>1.2120785266443335</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7176403578039845</v>
+        <v>1.1747156978068798</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2035980884610018</v>
+        <v>1.0614058863924769</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.176660464056507</v>
+        <v>1.0524413548375706</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2612344230749442</v>
+        <v>1.0619182485971845</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95069520159160137</v>
+        <v>0.99924033436634618</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1793271201979112</v>
+        <v>1.0690214909014535</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0084787350054525</v>
+        <v>0.9777246598710464</v>
       </c>
       <c r="K20" s="7">
+        <f>SUM(L3:L7)/SUM(K3:K7)</f>
         <v>1</v>
       </c>
       <c r="L20" s="7">
+        <f>SUM(M3:M6)/SUM(L3:L6)</f>
         <v>1</v>
       </c>
       <c r="M20" s="7">
+        <f>SUM(N3:N5)/SUM(M3:M5)</f>
         <v>1</v>
       </c>
       <c r="N20" s="7">
+        <f>SUM(O3:O4)/SUM(N3:N4)</f>
         <v>1</v>
       </c>
       <c r="O20" s="7">
@@ -5633,39 +5895,39 @@
       </c>
       <c r="B21" s="4">
         <f ca="1">B20*C21</f>
-        <v>16.02199477580378</v>
+        <v>3.2384096322290477</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" ref="C21:P21" ca="1" si="1">C20*D21</f>
-        <v>6.6012238047728378</v>
+        <v>1.7640340813177275</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4689898946286082</v>
+        <v>1.4553793690261103</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0196252835277675</v>
+        <v>1.2389205079520194</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6779897732391638</v>
+        <v>1.1672448060024256</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4260611489013038</v>
+        <v>1.1090829913107827</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1306868277702926</v>
+        <v>1.0444146644771419</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1893263223348127</v>
+        <v>1.0452086735864625</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0084787350054525</v>
+        <v>0.9777246598710464</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="1"/>
@@ -5704,39 +5966,39 @@
       </c>
       <c r="B23" s="13">
         <f t="shared" ref="B23:K23" ca="1" si="2">SUM(OFFSET(C13:C17,-C19,0))-SUM(OFFSET(B13:B17,-C19,0))</f>
-        <v>83297</v>
+        <v>20835216.625329994</v>
       </c>
       <c r="C23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>121948</v>
+        <v>8956905.3231360018</v>
       </c>
       <c r="D23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>166311</v>
+        <v>8153680.1475279853</v>
       </c>
       <c r="E23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>70041</v>
+        <v>3376762.6318947077</v>
       </c>
       <c r="F23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>69780</v>
+        <v>3196796.3234260008</v>
       </c>
       <c r="G23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>101546</v>
+        <v>4243687.1105000079</v>
       </c>
       <c r="H23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>-17546</v>
+        <v>-49044.400500006974</v>
       </c>
       <c r="I23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>38926</v>
+        <v>3573267.7530000135</v>
       </c>
       <c r="J23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>933</v>
+        <v>-1005437.7870000079</v>
       </c>
       <c r="K23" s="13">
         <f t="shared" ca="1" si="2"/>
@@ -5754,14 +6016,8 @@
         <f>SUM(O3:O4)-SUM(N3:N4)</f>
         <v>0</v>
       </c>
-      <c r="O23" s="14">
-        <f>SUM(P3:P4)-SUM(O3:O4)</f>
-        <v>0</v>
-      </c>
-      <c r="P23" s="14">
-        <f>SUM(Q3)-SUM(P3)</f>
-        <v>0</v>
-      </c>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -5769,55 +6025,55 @@
       </c>
       <c r="B24" s="13">
         <f t="shared" ref="B24:K24" ca="1" si="3">SUM(OFFSET(C13:C17,-C19,0))</f>
-        <v>141664</v>
+        <v>45763758.200779989</v>
       </c>
       <c r="C24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>257007</v>
+        <v>51190814.926615998</v>
       </c>
       <c r="D24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>398058</v>
+        <v>54821954.663653992</v>
       </c>
       <c r="E24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>414057</v>
+        <v>58367624.750748701</v>
       </c>
       <c r="F24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>464775</v>
+        <v>64156249.665689997</v>
       </c>
       <c r="G24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>490262</v>
+        <v>72780624.227500007</v>
       </c>
       <c r="H24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>338322</v>
+        <v>64511465.285999991</v>
       </c>
       <c r="I24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>255993</v>
+        <v>55343632.408000007</v>
       </c>
       <c r="J24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>110973</v>
+        <v>44131371.850000001</v>
       </c>
       <c r="K24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>29140019.364999991</v>
       </c>
       <c r="L24" s="14">
         <f>SUM(M3:M6)</f>
-        <v>0</v>
+        <v>11872319.735999994</v>
       </c>
       <c r="M24" s="14">
         <f>SUM(N3:N6)</f>
-        <v>0</v>
+        <v>4271606.5979999993</v>
       </c>
       <c r="N24" s="14">
         <f>SUM(O3:O6)</f>
-        <v>0</v>
+        <v>1025162.2289999999</v>
       </c>
       <c r="O24" s="14">
         <f>SUM(P3:P6)</f>
@@ -5834,39 +6090,39 @@
       </c>
       <c r="B25" s="3">
         <f ca="1">IF(B24=0,0,B23/B24)</f>
-        <v>0.5879898915744296</v>
+        <v>0.45527765735321279</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25:P25" ca="1" si="4">IF(C24=0,0,C23/C24)</f>
-        <v>0.47449291264440269</v>
+        <v>0.1749709461741539</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.41780594787694253</v>
+        <v>0.14873019755593891</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.16915786956868256</v>
+        <v>5.7853350145988129E-2</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.15013716314345651</v>
+        <v>4.9828291711003947E-2</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.20712598569744342</v>
+        <v>5.8307924060048658E-2</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-5.1861835765927136E-2</v>
+        <v>-7.6024316425890245E-4</v>
       </c>
       <c r="I25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.15205884535905279</v>
+        <v>6.4565110700675513E-2</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>8.4074504609229269E-3</v>
+        <v>-2.2782835539702534E-2</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -5918,39 +6174,39 @@
       </c>
       <c r="B27" s="6">
         <f ca="1">C27*(1-B25)</f>
-        <v>6.2414200852829373E-2</v>
+        <v>0.30879354793410868</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" ref="C27:P27" ca="1" si="5">D27*(1-C25)</f>
-        <v>0.15148706203188822</v>
+        <v>0.56688247159771599</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.2882683519915703</v>
+        <v>0.68710607095465781</v>
       </c>
       <c r="E27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.49514135525836567</v>
+        <v>0.80715428760884445</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.59595118870695873</v>
+        <v>0.85671831209495375</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.70123220225895699</v>
+        <v>0.90164578109536986</v>
       </c>
       <c r="H27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.88441819205764827</v>
+        <v>0.9574741087158356</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.8408121313895256</v>
+        <v>0.95674674854033093</v>
       </c>
       <c r="J27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99159254953907705</v>
+        <v>1.0227828355397026</v>
       </c>
       <c r="K27" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -5986,39 +6242,39 @@
       </c>
       <c r="B28" s="4">
         <f ca="1">1/B27</f>
-        <v>16.02199477580378</v>
+        <v>3.2384096322290485</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" ref="C28:Q28" ca="1" si="6">1/C27</f>
-        <v>6.6012238047728378</v>
+        <v>1.764034081317728</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>3.4689898946286082</v>
+        <v>1.4553793690261108</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>2.0196252835277679</v>
+        <v>1.2389205079520196</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.6779897732391642</v>
+        <v>1.1672448060024259</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.4260611489013042</v>
+        <v>1.1090829913107827</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.1306868277702928</v>
+        <v>1.0444146644771419</v>
       </c>
       <c r="I28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.1893263223348129</v>
+        <v>1.0452086735864625</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0084787350054525</v>
+        <v>0.97772465987104629</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" ca="1" si="6"/>
@@ -6055,39 +6311,39 @@
       </c>
       <c r="B29" s="4">
         <f ca="1">B28/C28</f>
-        <v>2.4271249164767759</v>
+        <v>1.8357976563638536</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" ref="C29:P29" ca="1" si="7">C28/D28</f>
-        <v>1.9029239073293893</v>
+        <v>1.2120785266443335</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.7176403578039841</v>
+        <v>1.1747156978068798</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.2035980884610018</v>
+        <v>1.0614058863924769</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.176660464056507</v>
+        <v>1.0524413548375708</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.2612344230749444</v>
+        <v>1.0619182485971845</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>0.95069520159160137</v>
+        <v>0.99924033436634607</v>
       </c>
       <c r="I29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.1793271201979114</v>
+        <v>1.0690214909014537</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0084787350054525</v>
+        <v>0.97772465987104629</v>
       </c>
       <c r="K29" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -6187,55 +6443,55 @@
       </c>
       <c r="B35" s="13">
         <f ca="1">B24*LN(B2)^1.67/1000</f>
-        <v>647.77969550179216</v>
+        <v>209261.58623446256</v>
       </c>
       <c r="C35" s="13">
         <f t="shared" ref="C35:P35" ca="1" si="9">C24*LN(C2)^1.67/1000</f>
-        <v>1772.3693789563176</v>
+        <v>353021.64088820224</v>
       </c>
       <c r="D35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>3354.6217797835648</v>
+        <v>462010.36814986973</v>
       </c>
       <c r="E35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>3969.7438792360731</v>
+        <v>559595.71049356146</v>
       </c>
       <c r="F35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>4893.1743199659668</v>
+        <v>675440.1878962497</v>
       </c>
       <c r="G35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>5551.0374903250449</v>
+        <v>824065.44593729847</v>
       </c>
       <c r="H35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>4064.0418810611654</v>
+        <v>774934.2245876044</v>
       </c>
       <c r="I35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>3231.3993337594065</v>
+        <v>698602.60589561716</v>
       </c>
       <c r="J35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>1461.699532320823</v>
+        <v>581283.78609050252</v>
       </c>
       <c r="K35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>398354.9878473148</v>
       </c>
       <c r="L35" s="13">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>167730.86732766757</v>
       </c>
       <c r="M35" s="13">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>62155.443859506195</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15320.344032166218</v>
       </c>
       <c r="O35" s="13">
         <f t="shared" si="9"/>
@@ -6572,39 +6828,39 @@
       </c>
       <c r="B41" s="4">
         <f t="shared" ref="B41" ca="1" si="11">B25*B35^0.5</f>
-        <v>14.965234465959577</v>
+        <v>208.26730364953627</v>
       </c>
       <c r="C41" s="4">
         <f ca="1">C25*C35^0.5</f>
-        <v>19.975922708935432</v>
+        <v>103.9600799824121</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" ref="D41:P41" ca="1" si="12">D25*D35^0.5</f>
-        <v>24.198943159099745</v>
+        <v>101.09391504775282</v>
       </c>
       <c r="E41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>10.657944410853693</v>
+        <v>43.277852394421004</v>
       </c>
       <c r="F41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>10.502278953134255</v>
+        <v>40.951465374792981</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>15.431980591671334</v>
+        <v>52.930796770546969</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>-3.3061836431180445</v>
+        <v>-0.6692447064628404</v>
       </c>
       <c r="I41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>8.6438456640790307</v>
+        <v>53.965101797379837</v>
       </c>
       <c r="J41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>0.32143515329023614</v>
+        <v>-17.370082445222359</v>
       </c>
       <c r="K41" s="4">
         <f t="shared" ca="1" si="12"/>
@@ -6639,55 +6895,55 @@
       </c>
       <c r="B42" s="4">
         <f t="shared" ref="B42:P42" ca="1" si="13">B38*B$35^0.5</f>
-        <v>-3.3207255402896618</v>
+        <v>-59.684845419644731</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-4.2991522140142111</v>
+        <v>-60.674522529821829</v>
       </c>
       <c r="D42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-4.8002287548833795</v>
+        <v>-56.333406496969026</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-4.3803795927870626</v>
+        <v>-52.007705229474006</v>
       </c>
       <c r="F42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-4.1647296402440181</v>
+        <v>-48.931093164270507</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-3.8495316139478342</v>
+        <v>-46.903112373619663</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.8834198479860493</v>
+        <v>-39.816329067693161</v>
       </c>
       <c r="I42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.2634331290621419</v>
+        <v>-33.280316919357823</v>
       </c>
       <c r="J42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.3446089230371967</v>
+        <v>-26.813965087779003</v>
       </c>
       <c r="K42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>-19.636567394483514</v>
       </c>
       <c r="L42" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-11.271881854348004</v>
       </c>
       <c r="M42" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-6.0611982170057699</v>
       </c>
       <c r="N42" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-2.6504665178754721</v>
       </c>
       <c r="O42" s="4">
         <f t="shared" si="13"/>
@@ -6705,55 +6961,55 @@
       </c>
       <c r="B43" s="4">
         <f t="shared" ref="B43:P43" ca="1" si="14">B37*B$35^0.5</f>
-        <v>8.6737566915774931</v>
+        <v>155.89720410897144</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>9.7634052549058801</v>
+        <v>137.79227220090453</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>10.410492904159351</v>
+        <v>122.17303769267312</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>9.2702387260857844</v>
+        <v>110.06439804144182</v>
       </c>
       <c r="F43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>8.6770469331750686</v>
+        <v>101.94596733848499</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>7.9323593170975668</v>
+        <v>96.648729702521649</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>5.8927320414897499</v>
+        <v>81.371069924337419</v>
       </c>
       <c r="I43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>4.5960755990460909</v>
+        <v>67.578251178536064</v>
       </c>
       <c r="J43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>2.7163819814959931</v>
+        <v>54.169632797305617</v>
       </c>
       <c r="K43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
+        <v>39.505708172561363</v>
       </c>
       <c r="L43" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>22.600882033836989</v>
       </c>
       <c r="M43" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>12.119940307321546</v>
       </c>
       <c r="N43" s="4">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>5.2883559597325691</v>
       </c>
       <c r="O43" s="4">
         <f t="shared" si="14"/>
@@ -6770,55 +7026,55 @@
       </c>
       <c r="B44" s="4">
         <f t="shared" ref="B44:P44" ca="1" si="15">B36*B$35^0.5</f>
-        <v>10.242443742513418</v>
+        <v>184.09189921730066</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>13.246949173742737</v>
+        <v>186.95600343565818</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>16.162631715790031</v>
+        <v>189.67764850375849</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>16.275544294736648</v>
+        <v>193.23752478523119</v>
       </c>
       <c r="F44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>17.084841563501527</v>
+        <v>200.7285097602429</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>17.421347121587257</v>
+        <v>212.26359040227786</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>14.387829869036734</v>
+        <v>198.67747287502297</v>
       </c>
       <c r="I44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>12.454220436959993</v>
+        <v>183.12023350886997</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>8.1655505629995773</v>
+        <v>162.83603653633341</v>
       </c>
       <c r="K44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>131.83389754161902</v>
       </c>
       <c r="L44" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>83.875937893257216</v>
       </c>
       <c r="M44" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>50.16484932377918</v>
       </c>
       <c r="N44" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>24.51067459115627</v>
       </c>
       <c r="O44" s="4">
         <f t="shared" si="15"/>
@@ -6846,15 +7102,15 @@
       </c>
       <c r="B48" s="3" cm="1">
         <f t="array" aca="1" ref="B48:E48" ca="1">LINEST(B41:P41,B42:P44,FALSE)</f>
-        <v>-1.3682924138527504</v>
+        <v>-0.17229740473953556</v>
       </c>
       <c r="C48" s="3">
         <f ca="1"/>
-        <v>0.45315273761002012</v>
+        <v>4.453868716666058</v>
       </c>
       <c r="D48" s="3">
         <f ca="1"/>
-        <v>-7.7405827708819173</v>
+        <v>7.6548097524843204</v>
       </c>
       <c r="E48" s="3">
         <f ca="1"/>
@@ -6878,43 +7134,43 @@
       </c>
       <c r="B51" s="10" cm="1">
         <f t="array" aca="1" ref="B51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*B36:B38)))</f>
-        <v>0.61372489853546219</v>
+        <v>0.44977692503363254</v>
       </c>
       <c r="C51" s="10" cm="1">
         <f t="array" aca="1" ref="C51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*C36:C38)))</f>
-        <v>0.46500669008571971</v>
+        <v>0.19699318316734493</v>
       </c>
       <c r="D51" s="10" cm="1">
         <f t="array" aca="1" ref="D51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*D36:D38)))</f>
-        <v>0.3411466349810881</v>
+        <v>0.11805003284714632</v>
       </c>
       <c r="E51" s="10" cm="1">
         <f t="array" aca="1" ref="E51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*E36:E38)))</f>
-        <v>0.2513704301742129</v>
+        <v>7.8615169559021481E-2</v>
       </c>
       <c r="F51" s="10" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*F36:F38)))</f>
-        <v>0.18287603099390831</v>
+        <v>5.4645801958335238E-2</v>
       </c>
       <c r="G51" s="10" cm="1">
         <f t="array" aca="1" ref="G51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*G36:G38)))</f>
-        <v>0.12824179283145642</v>
+        <v>3.8394618252735491E-2</v>
       </c>
       <c r="H51" s="10" cm="1">
         <f t="array" aca="1" ref="H51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*H36:H38)))</f>
-        <v>8.3182943430011036E-2</v>
+        <v>2.6579499208066126E-2</v>
       </c>
       <c r="I51" s="10" cm="1">
         <f t="array" aca="1" ref="I51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*I36:I38)))</f>
-        <v>4.5069617662137462E-2</v>
+        <v>1.75623270502E-2</v>
       </c>
       <c r="J51" s="10" cm="1">
         <f t="array" aca="1" ref="J51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*J36:J38)))</f>
-        <v>1.2192130113126476E-2</v>
+        <v>1.0430482117881723E-2</v>
       </c>
       <c r="K51" s="10" cm="1">
         <f t="array" aca="1" ref="K51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*K36:K38)))</f>
-        <v>0</v>
+        <v>4.6334383824151726E-3</v>
       </c>
       <c r="L51" s="10" cm="1">
         <f t="array" aca="1" ref="L51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*L36:L38)))</f>
@@ -6985,43 +7241,43 @@
       </c>
       <c r="B52" s="6">
         <f ca="1">C52*(1-B51)</f>
-        <v>6.2793065320503494E-2</v>
+        <v>0.30744634368928597</v>
       </c>
       <c r="C52" s="6">
         <f t="shared" ref="C52:Z52" ca="1" si="16">D52*(1-C51)</f>
-        <v>0.16256047848392902</v>
+        <v>0.55876672149396622</v>
       </c>
       <c r="D52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.30385516131028889</v>
+        <v>0.69584306108127603</v>
       </c>
       <c r="E52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.46118784154888087</v>
+        <v>0.78898246725675891</v>
       </c>
       <c r="F52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.61604278021799685</v>
+        <v>0.85630069129654407</v>
       </c>
       <c r="G52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.75391593391553569</v>
+        <v>0.90579879273863884</v>
       </c>
       <c r="H52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.86482229558152635</v>
+        <v>0.94196518648094141</v>
       </c>
       <c r="I52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.94328774686742167</v>
+        <v>0.96768579017454248</v>
       </c>
       <c r="J52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.98780786988687352</v>
+        <v>0.98498440849589519</v>
       </c>
       <c r="K52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>0.99536656161758486</v>
       </c>
       <c r="L52" s="6">
         <f t="shared" ca="1" si="16"/>
@@ -7093,43 +7349,43 @@
       </c>
       <c r="B53" s="4">
         <f ca="1">1/B52</f>
-        <v>15.925325430377981</v>
+        <v>3.2526000732362861</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" ref="C53:Z53" ca="1" si="17">1/C52</f>
-        <v>6.1515566964750388</v>
+        <v>1.7896556139319015</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>3.2910416781725367</v>
+        <v>1.4371056577701473</v>
       </c>
       <c r="E53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>2.1683138840814626</v>
+        <v>1.2674552876655618</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.6232638902871868</v>
+        <v>1.1678140753172552</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.3264078327757352</v>
+        <v>1.1039979386333121</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.1563069142748883</v>
+        <v>1.0616103592276791</v>
       </c>
       <c r="I53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0601219016370296</v>
+        <v>1.0333932875253122</v>
       </c>
       <c r="J53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0123426128549904</v>
+        <v>1.0152444966383114</v>
       </c>
       <c r="K53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>1.0046550070708475</v>
       </c>
       <c r="L53" s="4">
         <f t="shared" ca="1" si="17"/>
@@ -7198,43 +7454,43 @@
       </c>
       <c r="B54" s="4">
         <f ca="1">B53/C53</f>
-        <v>2.5888285219745275</v>
+        <v>1.8174446792532741</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" ref="C54:Y54" ca="1" si="18">C53/D53</f>
-        <v>1.8691822523168107</v>
+        <v>1.2453194406796648</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.5177884080037989</v>
+        <v>1.1338511675761382</v>
       </c>
       <c r="E54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.3357741135348276</v>
+        <v>1.0853228390154808</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.22380451183723</v>
+        <v>1.0578045795655597</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.1471070668184284</v>
+        <v>1.0399276241393027</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0907301438535801</v>
+        <v>1.0273052593267167</v>
       </c>
       <c r="I54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.047196757476496</v>
+        <v>1.0178762760567481</v>
       </c>
       <c r="J54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0123426128549904</v>
+        <v>1.0105404238200517</v>
       </c>
       <c r="K54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>1.0046550070708475</v>
       </c>
       <c r="L54" s="4">
         <f t="shared" ca="1" si="18"/>
@@ -7312,11 +7568,11 @@
       </c>
       <c r="B59" s="4" cm="1">
         <f t="array" aca="1" ref="B59:C59" ca="1">LINEST(LN(IF(B20:P20&lt;=1,1.0001,B20:P20)-1),LN(B2:P2))</f>
-        <v>-4.4453777188792811</v>
+        <v>-4.0921201011967527</v>
       </c>
       <c r="C59" s="4">
         <f ca="1"/>
-        <v>14.267413127921735</v>
+        <v>11.889609557632173</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.35">
@@ -7330,103 +7586,103 @@
       </c>
       <c r="B62" s="4">
         <f ca="1">EXP($C$59+$B$59*LN(B2))+1</f>
-        <v>26.054776135765458</v>
+        <v>6.5905244743229829</v>
       </c>
       <c r="C62" s="4">
         <f t="shared" ref="C62:Z62" ca="1" si="19">EXP($C$59+$B$59*LN(C2))+1</f>
-        <v>2.1500017235279847</v>
+        <v>1.3277944957769152</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.1896296885437576</v>
+        <v>1.0623756487948866</v>
       </c>
       <c r="E62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0527845053155145</v>
+        <v>1.0192198839223674</v>
       </c>
       <c r="F62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0195751384879448</v>
+        <v>1.0077122899381779</v>
       </c>
       <c r="G62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0087039080882505</v>
+        <v>1.0036573302629095</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0043864231943886</v>
+        <v>1.001946300418612</v>
       </c>
       <c r="I62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0024227824571046</v>
+        <v>1.0011269375866538</v>
       </c>
       <c r="J62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0014352320923703</v>
+        <v>1.0006959492942842</v>
       </c>
       <c r="K62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0008984890895634</v>
+        <v>1.0004522019719584</v>
       </c>
       <c r="L62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0005881751710726</v>
+        <v>1.000306160115392</v>
       </c>
       <c r="M62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0003995050384278</v>
+        <v>1.0002144436957439</v>
       </c>
       <c r="N62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0002798926978369</v>
+        <v>1.0001545477082883</v>
       </c>
       <c r="O62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0002013346360126</v>
+        <v>1.0001141192686447</v>
       </c>
       <c r="P62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0001481564790105</v>
+        <v>1.0000860490086034</v>
       </c>
       <c r="Q62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0001112045059315</v>
+        <v>1.000066076794706</v>
       </c>
       <c r="R62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000849337515372</v>
+        <v>1.0000515593921184</v>
       </c>
       <c r="S62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000658764369295</v>
+        <v>1.0000408062515518</v>
       </c>
       <c r="T62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000518021471323</v>
+        <v>1.0000327068890822</v>
       </c>
       <c r="U62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000412402009089</v>
+        <v>1.0000265143848432</v>
       </c>
       <c r="V62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000331991018265</v>
+        <v>1.0000217156282776</v>
       </c>
       <c r="W62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000269969468818</v>
+        <v>1.0000179513748868</v>
       </c>
       <c r="X62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000221562341034</v>
+        <v>1.0000149657574713</v>
       </c>
       <c r="Y62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000183370819304</v>
+        <v>1.0000125736795253</v>
       </c>
       <c r="Z62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000152939321727</v>
+        <v>1.0000106393266612</v>
       </c>
     </row>
   </sheetData>
@@ -7436,20 +7692,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6AC979-46A0-45AC-AD4D-731805EBF10B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E14914A-8E2A-4748-9C7B-BA3BA6166CC6}">
   <dimension ref="A1:AB62"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.7265625" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="12" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -7548,397 +7806,179 @@
       <c r="A4" s="2">
         <v>2013</v>
       </c>
-      <c r="B4" s="13">
-        <v>387026.80900000001</v>
-      </c>
-      <c r="C4" s="13">
-        <v>463552.06300000002</v>
-      </c>
-      <c r="D4" s="13">
-        <v>485844.29399999999</v>
-      </c>
-      <c r="E4" s="13">
-        <v>778173.73400000005</v>
-      </c>
-      <c r="F4" s="13">
-        <v>909494.57299999997</v>
-      </c>
-      <c r="G4" s="13">
-        <v>1026309.7130000002</v>
-      </c>
-      <c r="H4" s="13">
-        <v>990261.68800000008</v>
-      </c>
-      <c r="I4" s="13">
-        <v>990261.68800000008</v>
-      </c>
-      <c r="J4" s="13">
-        <v>1025162.2289999999</v>
-      </c>
-      <c r="K4" s="13">
-        <v>1025162.2289999999</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1025162.2289999999</v>
-      </c>
-      <c r="M4" s="13">
-        <v>1025162.2289999999</v>
-      </c>
-      <c r="N4" s="13">
-        <v>1025162.2289999999</v>
-      </c>
-      <c r="O4" s="13">
-        <v>1025162.2289999999</v>
-      </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2014</v>
       </c>
-      <c r="B5" s="13">
-        <v>721554.38100000017</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1017504.4859999997</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1986074.2079999994</v>
-      </c>
-      <c r="E5" s="13">
-        <v>2575477.6020000004</v>
-      </c>
-      <c r="F5" s="13">
-        <v>3477456.1260000006</v>
-      </c>
-      <c r="G5" s="13">
-        <v>3247546.0949999993</v>
-      </c>
-      <c r="H5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="I5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="J5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="K5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="L5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="M5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="N5" s="13">
-        <v>3246444.3689999995</v>
-      </c>
-      <c r="O5" s="13"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2015</v>
       </c>
-      <c r="B6" s="13">
-        <v>3512563.7219999991</v>
-      </c>
-      <c r="C6" s="13">
-        <v>5266562.3999999976</v>
-      </c>
-      <c r="D6" s="13">
-        <v>6351170.7869999949</v>
-      </c>
-      <c r="E6" s="13">
-        <v>7008749.8739999942</v>
-      </c>
-      <c r="F6" s="13">
-        <v>7839785.8529999955</v>
-      </c>
-      <c r="G6" s="13">
-        <v>7643692.7009999957</v>
-      </c>
-      <c r="H6" s="13">
-        <v>7600920.3179999935</v>
-      </c>
-      <c r="I6" s="13">
-        <v>7601336.3969999934</v>
-      </c>
-      <c r="J6" s="13">
-        <v>8654880</v>
-      </c>
-      <c r="K6" s="13">
-        <v>7600713.1379999937</v>
-      </c>
-      <c r="L6" s="13">
-        <v>7600713.1379999937</v>
-      </c>
-      <c r="M6" s="13">
-        <v>7600713.1379999937</v>
-      </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2016</v>
       </c>
-      <c r="B7" s="13">
-        <v>4870653.2379999934</v>
-      </c>
-      <c r="C7" s="13">
-        <v>8588861.5669999961</v>
-      </c>
-      <c r="D7" s="13">
-        <v>14932191.723000005</v>
-      </c>
-      <c r="E7" s="13">
-        <v>17189503.470999993</v>
-      </c>
-      <c r="F7" s="13">
-        <v>17301048.222999994</v>
-      </c>
-      <c r="G7" s="13">
-        <v>17271026.528999999</v>
-      </c>
-      <c r="H7" s="13">
-        <v>17271833.025999997</v>
-      </c>
-      <c r="I7" s="13">
-        <v>17266960.128999997</v>
-      </c>
-      <c r="J7" s="13">
-        <v>17267699.628999997</v>
-      </c>
-      <c r="K7" s="13">
-        <v>17267699.628999997</v>
-      </c>
-      <c r="L7" s="13">
-        <v>17267699.628999997</v>
-      </c>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2017</v>
       </c>
-      <c r="B8" s="13">
-        <v>5768068.1924999971</v>
-      </c>
-      <c r="C8" s="13">
-        <v>10037063.895000013</v>
-      </c>
-      <c r="D8" s="13">
-        <v>10652257.732500013</v>
-      </c>
-      <c r="E8" s="13">
-        <v>12006271.860000012</v>
-      </c>
-      <c r="F8" s="13">
-        <v>12089139.85500001</v>
-      </c>
-      <c r="G8" s="13">
-        <v>12769212.660000011</v>
-      </c>
-      <c r="H8" s="13">
-        <v>14135430.285000011</v>
-      </c>
-      <c r="I8" s="13">
-        <v>14025377.182500012</v>
-      </c>
-      <c r="J8" s="13">
-        <v>14942623.410000008</v>
-      </c>
-      <c r="K8" s="13">
-        <v>14991352.485000009</v>
-      </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2018</v>
       </c>
-      <c r="B9" s="13">
-        <v>5019038.7225000057</v>
-      </c>
-      <c r="C9" s="13">
-        <v>7594422.4050000068</v>
-      </c>
-      <c r="D9" s="13">
-        <v>8270724.5700000059</v>
-      </c>
-      <c r="E9" s="13">
-        <v>8827020.8699999973</v>
-      </c>
-      <c r="F9" s="13">
-        <v>9476244.7874999959</v>
-      </c>
-      <c r="G9" s="13">
-        <v>9398204.8799999971</v>
-      </c>
-      <c r="H9" s="13">
-        <v>9247393.0574999955</v>
-      </c>
-      <c r="I9" s="13">
-        <v>9630246.577499995</v>
-      </c>
-      <c r="J9" s="13">
-        <v>11231985</v>
-      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>2019</v>
       </c>
       <c r="B10" s="13">
-        <v>4799936.1359999962</v>
+        <v>8347</v>
       </c>
       <c r="C10" s="13">
-        <v>9923861.3215200026</v>
+        <v>18022</v>
       </c>
       <c r="D10" s="13">
-        <v>11191566.177540002</v>
+        <v>43096</v>
       </c>
       <c r="E10" s="13">
-        <v>11744990.166240001</v>
+        <v>71537</v>
       </c>
       <c r="F10" s="13">
-        <v>11492856.698519999</v>
+        <v>74052</v>
       </c>
       <c r="G10" s="13">
-        <v>13545433</v>
+        <v>100813</v>
       </c>
       <c r="H10" s="13">
-        <v>16304933</v>
+        <v>105738</v>
       </c>
       <c r="I10" s="13">
-        <v>12414661.150740003</v>
+        <v>128602</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2020</v>
       </c>
       <c r="B11" s="13">
-        <v>5493944.7647999981</v>
+        <v>7700</v>
       </c>
       <c r="C11" s="13">
-        <v>9782584.9694000017</v>
+        <v>21502</v>
       </c>
       <c r="D11" s="13">
-        <v>11469778.782000007</v>
+        <v>52902</v>
       </c>
       <c r="E11" s="13">
-        <v>13748603.980399996</v>
+        <v>64383</v>
       </c>
       <c r="F11" s="13">
-        <v>15373592.092799991</v>
+        <v>69693</v>
       </c>
       <c r="G11" s="13">
-        <v>15553060.047999991</v>
+        <v>93042</v>
       </c>
       <c r="H11" s="13">
-        <v>15821034.859000001</v>
+        <v>112434</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>2021</v>
       </c>
       <c r="B12" s="13">
-        <v>3957732.8453999995</v>
+        <v>8223</v>
       </c>
       <c r="C12" s="13">
-        <v>7073422.3987300014</v>
+        <v>23181</v>
       </c>
       <c r="D12" s="13">
-        <v>9012357.8970860001</v>
+        <v>49502</v>
       </c>
       <c r="E12" s="13">
-        <v>12220604.864725998</v>
+        <v>67965</v>
       </c>
       <c r="F12" s="13">
-        <v>12527619.908443999</v>
+        <v>72611</v>
       </c>
       <c r="G12" s="13">
-        <v>12890339.077689998</v>
+        <v>138076</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>2022</v>
       </c>
       <c r="B13" s="13">
-        <v>4420890.5543999989</v>
+        <v>12122</v>
       </c>
       <c r="C13" s="13">
-        <v>6193275.3660000023</v>
+        <v>26156</v>
       </c>
       <c r="D13" s="13">
-        <v>8009139.5616000025</v>
+        <v>48834</v>
       </c>
       <c r="E13" s="13">
-        <v>8449642.2374880016</v>
+        <v>82909</v>
       </c>
       <c r="F13" s="13">
-        <v>9497311.2634847071</v>
+        <v>85302</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2023</v>
       </c>
       <c r="B14" s="13">
-        <v>3503613.7829999998</v>
+        <v>7596</v>
       </c>
       <c r="C14" s="13">
-        <v>6135103.6164999977</v>
+        <v>19404</v>
       </c>
       <c r="D14" s="13">
-        <v>6985432.0978999939</v>
+        <v>76420</v>
       </c>
       <c r="E14" s="13">
-        <v>8658113.4147999957</v>
+        <v>111264</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -7946,23 +7986,19 @@
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2024</v>
       </c>
       <c r="B15" s="13">
-        <v>7754842.6332499953</v>
+        <v>10264</v>
       </c>
       <c r="C15" s="13">
-        <v>13049523.252849992</v>
+        <v>44816</v>
       </c>
       <c r="D15" s="13">
-        <v>15714106.588029997</v>
+        <v>89632</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -7971,20 +8007,16 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2025</v>
       </c>
       <c r="B16" s="13">
-        <v>5291461.7594000008</v>
+        <v>20162</v>
       </c>
       <c r="C16" s="13">
-        <v>13312433.566699998</v>
+        <v>28107</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -7994,17 +8026,13 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>2026</v>
       </c>
       <c r="B17" s="13">
-        <v>6373903.717600002</v>
+        <v>10682</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -8015,22 +8043,9 @@
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
@@ -8088,54 +8103,48 @@
       </c>
       <c r="B20" s="4">
         <f ca="1">SUM(OFFSET(C13:C17,-B19-1,0))/SUM(OFFSET(B13:B17,-B19-1,0))</f>
-        <v>1.8357976563638536</v>
+        <v>2.4271249164767763</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" ref="C20:J20" ca="1" si="0">SUM(OFFSET(D13:D17,-C19-1,0))/SUM(OFFSET(C13:C17,-C19-1,0))</f>
-        <v>1.2120785266443335</v>
+        <v>2.349269578480516</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1747156978068798</v>
+        <v>1.4701832659905301</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0614058863924769</v>
+        <v>1.0518281414534474</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0524413548375706</v>
+        <v>1.5341890217974079</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0619182485971845</v>
+        <v>1.1254391168656985</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94389870421798472</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0690214909014535</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9777246598710464</v>
+        <v>1.2162325748548299</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7">
+        <v>1</v>
       </c>
       <c r="K20" s="7">
-        <f>SUM(L3:L7)/SUM(K3:K7)</f>
         <v>1</v>
       </c>
       <c r="L20" s="7">
-        <f>SUM(M3:M6)/SUM(L3:L6)</f>
         <v>1</v>
       </c>
       <c r="M20" s="7">
-        <f>SUM(N3:N5)/SUM(M3:M5)</f>
         <v>1</v>
       </c>
       <c r="N20" s="7">
-        <f>SUM(O3:O4)/SUM(N3:N4)</f>
         <v>1</v>
       </c>
       <c r="O20" s="7">
@@ -8152,39 +8161,39 @@
       </c>
       <c r="B21" s="4">
         <f ca="1">B20*C21</f>
-        <v>3.0590545141739307</v>
+        <v>18.516493734949638</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" ref="C21:P21" ca="1" si="1">C20*D21</f>
-        <v>1.666335341245053</v>
+        <v>7.6289825913979943</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3747750699439745</v>
+        <v>3.2473849154137278</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1703045021962275</v>
+        <v>2.2088300081594352</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1025984660532429</v>
+        <v>2.0999913589564243</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0476578680466364</v>
+        <v>1.3687957149479144</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98657111263566055</v>
+        <v>1.2162325748548299</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0452086735864625</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.9777246598710464</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="1"/>
@@ -8223,39 +8232,39 @@
       </c>
       <c r="B23" s="13">
         <f t="shared" ref="B23:K23" ca="1" si="2">SUM(OFFSET(C13:C17,-C19,0))-SUM(OFFSET(B13:B17,-C19,0))</f>
-        <v>20835216.625329994</v>
+        <v>83297</v>
       </c>
       <c r="C23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>8956905.3231360018</v>
+        <v>182231</v>
       </c>
       <c r="D23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>8153680.1475279853</v>
+        <v>127304</v>
       </c>
       <c r="E23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3376762.6318947077</v>
+        <v>14864</v>
       </c>
       <c r="F23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3196796.3234260008</v>
+        <v>115575</v>
       </c>
       <c r="G23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>4243687.1105000079</v>
+        <v>24317</v>
       </c>
       <c r="H23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>-3621928.2497600019</v>
+        <v>22864</v>
       </c>
       <c r="I23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3573267.7530000135</v>
+        <v>0</v>
       </c>
       <c r="J23" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>-1005437.7870000079</v>
+        <v>0</v>
       </c>
       <c r="K23" s="13">
         <f t="shared" ca="1" si="2"/>
@@ -8273,8 +8282,14 @@
         <f>SUM(O3:O4)-SUM(N3:N4)</f>
         <v>0</v>
       </c>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
+      <c r="O23" s="14">
+        <f>SUM(P3:P4)-SUM(O3:O4)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="14">
+        <f>SUM(Q3)-SUM(P3)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -8282,55 +8297,55 @@
       </c>
       <c r="B24" s="13">
         <f t="shared" ref="B24:K24" ca="1" si="3">SUM(OFFSET(C13:C17,-C19,0))</f>
-        <v>45763758.200779989</v>
+        <v>141664</v>
       </c>
       <c r="C24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>51190814.926615998</v>
+        <v>317290</v>
       </c>
       <c r="D24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>54821954.663653992</v>
+        <v>398058</v>
       </c>
       <c r="E24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>58367624.750748701</v>
+        <v>301658</v>
       </c>
       <c r="F24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>64156249.665689997</v>
+        <v>331931</v>
       </c>
       <c r="G24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>72780624.227500007</v>
+        <v>218172</v>
       </c>
       <c r="H24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>60938581.436739996</v>
+        <v>128602</v>
       </c>
       <c r="I24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>55343632.408000007</v>
+        <v>0</v>
       </c>
       <c r="J24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>44131371.850000001</v>
+        <v>0</v>
       </c>
       <c r="K24" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>29140019.364999991</v>
+        <v>0</v>
       </c>
       <c r="L24" s="14">
         <f>SUM(M3:M6)</f>
-        <v>11872319.735999994</v>
+        <v>0</v>
       </c>
       <c r="M24" s="14">
         <f>SUM(N3:N6)</f>
-        <v>4271606.5979999993</v>
+        <v>0</v>
       </c>
       <c r="N24" s="14">
         <f>SUM(O3:O6)</f>
-        <v>1025162.2289999999</v>
+        <v>0</v>
       </c>
       <c r="O24" s="14">
         <f>SUM(P3:P6)</f>
@@ -8347,39 +8362,39 @@
       </c>
       <c r="B25" s="3">
         <f ca="1">IF(B24=0,0,B23/B24)</f>
-        <v>0.45527765735321279</v>
+        <v>0.5879898915744296</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25:P25" ca="1" si="4">IF(C24=0,0,C23/C24)</f>
-        <v>0.1749709461741539</v>
+        <v>0.57433578114658512</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.14873019755593891</v>
+        <v>0.31981269061292578</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>5.7853350145988129E-2</v>
+        <v>4.9274343793302346E-2</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4.9828291711003947E-2</v>
+        <v>0.34818983463430653</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>5.8307924060048658E-2</v>
+        <v>0.11145793227361898</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-5.9435716493005428E-2</v>
+        <v>0.17778883687656491</v>
       </c>
       <c r="I25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>6.4565110700675513E-2</v>
+        <v>0</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.2782835539702534E-2</v>
+        <v>0</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -8431,39 +8446,39 @@
       </c>
       <c r="B27" s="6">
         <f ca="1">C27*(1-B25)</f>
-        <v>0.32689839143649285</v>
+        <v>5.4005904914520265E-2</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" ref="C27:P27" ca="1" si="5">D27*(1-C25)</f>
-        <v>0.60011930086822718</v>
+        <v>0.13107907745490771</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.72739171800718827</v>
+        <v>0.30794008904010589</v>
       </c>
       <c r="E27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.85447846959775942</v>
+        <v>0.45272836583439752</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.90694847742669693</v>
+        <v>0.47619243561885072</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.95451008435082485</v>
+        <v>0.73056920698940975</v>
       </c>
       <c r="H27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0136116770421788</v>
+        <v>0.82221116312343512</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.95674674854033093</v>
+        <v>1</v>
       </c>
       <c r="J27" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0227828355397026</v>
+        <v>1</v>
       </c>
       <c r="K27" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -8499,39 +8514,39 @@
       </c>
       <c r="B28" s="4">
         <f ca="1">1/B27</f>
-        <v>3.0590545141739307</v>
+        <v>18.516493734949631</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" ref="C28:Q28" ca="1" si="6">1/C27</f>
-        <v>1.666335341245053</v>
+        <v>7.6289825913979925</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.3747750699439745</v>
+        <v>3.2473849154137278</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.1703045021962273</v>
+        <v>2.2088300081594352</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.1025984660532426</v>
+        <v>2.0999913589564243</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0476578680466362</v>
+        <v>1.3687957149479144</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0.98657111263566033</v>
+        <v>1.2162325748548297</v>
       </c>
       <c r="I28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0452086735864625</v>
+        <v>1</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0.97772465987104629</v>
+        <v>1</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" ca="1" si="6"/>
@@ -8568,39 +8583,39 @@
       </c>
       <c r="B29" s="4">
         <f ca="1">B28/C28</f>
-        <v>1.8357976563638536</v>
+        <v>2.4271249164767759</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" ref="C29:P29" ca="1" si="7">C28/D28</f>
-        <v>1.2120785266443335</v>
+        <v>2.3492695784805155</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.17471569780688</v>
+        <v>1.4701832659905301</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0614058863924769</v>
+        <v>1.0518281414534474</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0524413548375706</v>
+        <v>1.5341890217974079</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0619182485971845</v>
+        <v>1.1254391168656988</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>0.9438987042179845</v>
+        <v>1.2162325748548297</v>
       </c>
       <c r="I29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0690214909014537</v>
+        <v>1</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>0.97772465987104629</v>
+        <v>1</v>
       </c>
       <c r="K29" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8654,7 +8669,7 @@
       </c>
       <c r="H30" t="b">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="b">
         <f t="shared" ca="1" si="8"/>
@@ -8700,55 +8715,55 @@
       </c>
       <c r="B35" s="13">
         <f ca="1">B24*LN(B2)^1.67/1000</f>
-        <v>209261.58623446256</v>
+        <v>647.77969550179216</v>
       </c>
       <c r="C35" s="13">
         <f t="shared" ref="C35:P35" ca="1" si="9">C24*LN(C2)^1.67/1000</f>
-        <v>353021.64088820224</v>
+        <v>2188.0924653766242</v>
       </c>
       <c r="D35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>462010.36814986973</v>
+        <v>3354.6217797835648</v>
       </c>
       <c r="E35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>559595.71049356146</v>
+        <v>2892.1259612145072</v>
       </c>
       <c r="F35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>675440.1878962497</v>
+        <v>3494.5860797173332</v>
       </c>
       <c r="G35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>824065.44593729847</v>
+        <v>2470.2729384271997</v>
       </c>
       <c r="H35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>732015.49745913013</v>
+        <v>1544.8120843108875</v>
       </c>
       <c r="I35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>698602.60589561716</v>
+        <v>0</v>
       </c>
       <c r="J35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>581283.78609050252</v>
+        <v>0</v>
       </c>
       <c r="K35" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>398354.9878473148</v>
+        <v>0</v>
       </c>
       <c r="L35" s="13">
         <f t="shared" si="9"/>
-        <v>167730.86732766757</v>
+        <v>0</v>
       </c>
       <c r="M35" s="13">
         <f t="shared" si="9"/>
-        <v>62155.443859506195</v>
+        <v>0</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="9"/>
-        <v>15320.344032166218</v>
+        <v>0</v>
       </c>
       <c r="O35" s="13">
         <f t="shared" si="9"/>
@@ -9085,39 +9100,39 @@
       </c>
       <c r="B41" s="4">
         <f t="shared" ref="B41" ca="1" si="11">B25*B35^0.5</f>
-        <v>208.26730364953627</v>
+        <v>14.965234465959577</v>
       </c>
       <c r="C41" s="4">
         <f ca="1">C25*C35^0.5</f>
-        <v>103.9600799824121</v>
+        <v>26.865733911687808</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" ref="D41:P41" ca="1" si="12">D25*D35^0.5</f>
-        <v>101.09391504775282</v>
+        <v>18.523262201093342</v>
       </c>
       <c r="E41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>43.277852394421004</v>
+        <v>2.6498997932782942</v>
       </c>
       <c r="F41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>40.951465374792981</v>
+        <v>20.583250481607852</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>52.930796770546969</v>
+        <v>5.539664360370252</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>-50.851953389808521</v>
+        <v>6.9878297881032951</v>
       </c>
       <c r="I41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>53.965101797379837</v>
+        <v>0</v>
       </c>
       <c r="J41" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>-17.370082445222359</v>
+        <v>0</v>
       </c>
       <c r="K41" s="4">
         <f t="shared" ca="1" si="12"/>
@@ -9152,55 +9167,55 @@
       </c>
       <c r="B42" s="4">
         <f t="shared" ref="B42:P42" ca="1" si="13">B38*B$35^0.5</f>
-        <v>-59.684845419644731</v>
+        <v>-3.3207255402896618</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-60.674522529821829</v>
+        <v>-4.7768162775856284</v>
       </c>
       <c r="D42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-56.333406496969026</v>
+        <v>-4.8002287548833795</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-52.007705229474006</v>
+        <v>-3.7388591529261985</v>
       </c>
       <c r="F42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-48.931093164270507</v>
+        <v>-3.5195678438627258</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-46.903112373619663</v>
+        <v>-2.567989719228986</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-38.698036862077629</v>
+        <v>-1.7777333721812805</v>
       </c>
       <c r="I42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-33.280316919357823</v>
+        <v>0</v>
       </c>
       <c r="J42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-26.813965087779003</v>
+        <v>0</v>
       </c>
       <c r="K42" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-19.636567394483514</v>
+        <v>0</v>
       </c>
       <c r="L42" s="4">
         <f t="shared" si="13"/>
-        <v>-11.271881854348004</v>
+        <v>0</v>
       </c>
       <c r="M42" s="4">
         <f t="shared" si="13"/>
-        <v>-6.0611982170057699</v>
+        <v>0</v>
       </c>
       <c r="N42" s="4">
         <f t="shared" si="13"/>
-        <v>-2.6504665178754721</v>
+        <v>0</v>
       </c>
       <c r="O42" s="4">
         <f t="shared" si="13"/>
@@ -9218,55 +9233,55 @@
       </c>
       <c r="B43" s="4">
         <f t="shared" ref="B43:P43" ca="1" si="14">B37*B$35^0.5</f>
-        <v>155.89720410897144</v>
+        <v>8.6737566915774931</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>137.79227220090453</v>
+        <v>10.848183740568832</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>122.17303769267312</v>
+        <v>10.410492904159351</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>110.06439804144182</v>
+        <v>7.9125829569450339</v>
       </c>
       <c r="F43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>101.94596733848499</v>
+        <v>7.3328782427042007</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>96.648729702521649</v>
+        <v>5.2916092705227626</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>79.085660008614738</v>
+        <v>3.6330839613229085</v>
       </c>
       <c r="I43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>67.578251178536064</v>
+        <v>0</v>
       </c>
       <c r="J43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>54.169632797305617</v>
+        <v>0</v>
       </c>
       <c r="K43" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>39.505708172561363</v>
+        <v>0</v>
       </c>
       <c r="L43" s="4">
         <f t="shared" si="14"/>
-        <v>22.600882033836989</v>
+        <v>0</v>
       </c>
       <c r="M43" s="4">
         <f t="shared" si="14"/>
-        <v>12.119940307321546</v>
+        <v>0</v>
       </c>
       <c r="N43" s="4">
         <f t="shared" si="14"/>
-        <v>5.2883559597325691</v>
+        <v>0</v>
       </c>
       <c r="O43" s="4">
         <f t="shared" si="14"/>
@@ -9283,55 +9298,55 @@
       </c>
       <c r="B44" s="4">
         <f t="shared" ref="B44:P44" ca="1" si="15">B36*B$35^0.5</f>
-        <v>184.09189921730066</v>
+        <v>10.242443742513418</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>186.95600343565818</v>
+        <v>14.71877228147722</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>189.67764850375849</v>
+        <v>16.162631715790031</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>193.23752478523119</v>
+        <v>13.891939377909981</v>
       </c>
       <c r="F44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>200.7285097602429</v>
+        <v>14.438214284869201</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>212.26359040227786</v>
+        <v>11.621632133441629</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>193.09736354425581</v>
+        <v>8.8706212275393117</v>
       </c>
       <c r="I44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>183.12023350886997</v>
+        <v>0</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>162.83603653633341</v>
+        <v>0</v>
       </c>
       <c r="K44" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>131.83389754161902</v>
+        <v>0</v>
       </c>
       <c r="L44" s="4">
         <f t="shared" si="15"/>
-        <v>83.875937893257216</v>
+        <v>0</v>
       </c>
       <c r="M44" s="4">
         <f t="shared" si="15"/>
-        <v>50.16484932377918</v>
+        <v>0</v>
       </c>
       <c r="N44" s="4">
         <f t="shared" si="15"/>
-        <v>24.51067459115627</v>
+        <v>0</v>
       </c>
       <c r="O44" s="4">
         <f t="shared" si="15"/>
@@ -9359,15 +9374,15 @@
       </c>
       <c r="B48" s="3" cm="1">
         <f t="array" aca="1" ref="B48:E48" ca="1">LINEST(B41:P41,B42:P44,FALSE)</f>
-        <v>-0.26057402094040738</v>
+        <v>-0.69281106201378784</v>
       </c>
       <c r="C48" s="3">
         <f ca="1"/>
-        <v>4.535560927160426</v>
+        <v>1.7011703479204645</v>
       </c>
       <c r="D48" s="3">
         <f ca="1"/>
-        <v>7.5765056453507409</v>
+        <v>-2.7337306258456024</v>
       </c>
       <c r="E48" s="3">
         <f ca="1"/>
@@ -9391,51 +9406,51 @@
       </c>
       <c r="B51" s="10" cm="1">
         <f t="array" aca="1" ref="B51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*B36:B38)))</f>
-        <v>0.4523086614238685</v>
+        <v>0.65762008437232755</v>
       </c>
       <c r="C51" s="10" cm="1">
         <f t="array" aca="1" ref="C51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*C36:C38)))</f>
-        <v>0.19615800933867078</v>
+        <v>0.45568946563879309</v>
       </c>
       <c r="D51" s="10" cm="1">
         <f t="array" aca="1" ref="D51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*D36:D38)))</f>
-        <v>0.11458919448274218</v>
+        <v>0.33900570309956091</v>
       </c>
       <c r="E51" s="10" cm="1">
         <f t="array" aca="1" ref="E51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*E36:E38)))</f>
-        <v>7.3275321194502196E-2</v>
+        <v>0.26139067984132835</v>
       </c>
       <c r="F51" s="10" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*F36:F38)))</f>
-        <v>4.7880668113087221E-2</v>
+        <v>0.20456848387426382</v>
       </c>
       <c r="G51" s="10" cm="1">
         <f t="array" aca="1" ref="G51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*G36:G38)))</f>
-        <v>3.0496501082514726E-2</v>
+        <v>0.16036681061342339</v>
       </c>
       <c r="H51" s="10" cm="1">
         <f t="array" aca="1" ref="H51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*H36:H38)))</f>
-        <v>1.7749123673486578E-2</v>
+        <v>0.12453343702608474</v>
       </c>
       <c r="I51" s="10" cm="1">
         <f t="array" aca="1" ref="I51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*I36:I38)))</f>
-        <v>7.9447191832019426E-3</v>
+        <v>9.4605763037713661E-2</v>
       </c>
       <c r="J51" s="10" cm="1">
         <f t="array" aca="1" ref="J51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*J36:J38)))</f>
-        <v>1.3466506591580663E-4</v>
+        <v>6.9042449727691579E-2</v>
       </c>
       <c r="K51" s="10" cm="1">
         <f t="array" aca="1" ref="K51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*K36:K38)))</f>
-        <v>0</v>
+        <v>4.68206755601909E-2</v>
       </c>
       <c r="L51" s="10" cm="1">
         <f t="array" aca="1" ref="L51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*L36:L38)))</f>
-        <v>0</v>
+        <v>2.7230063538423166E-2</v>
       </c>
       <c r="M51" s="10" cm="1">
         <f t="array" aca="1" ref="M51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*M36:M38)))</f>
-        <v>0</v>
+        <v>9.7589521470070328E-3</v>
       </c>
       <c r="N51" s="10" cm="1">
         <f t="array" aca="1" ref="N51" ca="1">MAX(0,MIN(1,SUM(TRANSPOSE($B$48:$D$48)*N36:N38)))</f>
@@ -9498,51 +9513,51 @@
       </c>
       <c r="B52" s="6">
         <f ca="1">C52*(1-B51)</f>
-        <v>0.32489474129072171</v>
+        <v>4.1171126874848328E-2</v>
       </c>
       <c r="C52" s="6">
         <f t="shared" ref="C52:Z52" ca="1" si="16">D52*(1-C51)</f>
-        <v>0.59320774021252831</v>
+        <v>0.12024983065776747</v>
       </c>
       <c r="D52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.73796560406665257</v>
+        <v>0.22092137312552754</v>
       </c>
       <c r="E52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.83347255247865693</v>
+        <v>0.33422583850039383</v>
       </c>
       <c r="F52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.8993745084602276</v>
+        <v>0.45250693347410481</v>
       </c>
       <c r="G52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.9446027176843943</v>
+        <v>0.56888232902576585</v>
       </c>
       <c r="H52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.97431594495440765</v>
+        <v>0.67753673415575999</v>
       </c>
       <c r="I52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.99192168562701477</v>
+        <v>0.77391503320721045</v>
       </c>
       <c r="J52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>0.99986533493408425</v>
+        <v>0.85478237171444182</v>
       </c>
       <c r="K52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>0.91817545436353665</v>
       </c>
       <c r="L52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>0.96327672120160124</v>
       </c>
       <c r="M52" s="6">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>0.99024104785299294</v>
       </c>
       <c r="N52" s="6">
         <f t="shared" ca="1" si="16"/>
@@ -9606,51 +9621,51 @@
       </c>
       <c r="B53" s="4">
         <f ca="1">1/B52</f>
-        <v>3.0779199319363002</v>
+        <v>24.288866395126668</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" ref="C53:Z53" ca="1" si="17">1/C52</f>
-        <v>1.6857500875523479</v>
+        <v>8.3160200270552771</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.3550767061355893</v>
+        <v>4.5264973046849564</v>
       </c>
       <c r="E53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.1997995579171845</v>
+        <v>2.9919889033319658</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.1118838599417813</v>
+        <v>2.209910889812313</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0586461178636104</v>
+        <v>1.7578327695861826</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.026361115384183</v>
+        <v>1.4759347347358858</v>
       </c>
       <c r="I53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0081441050135715</v>
+        <v>1.2921315093930432</v>
       </c>
       <c r="J53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0001346832030382</v>
+        <v>1.1698884220018417</v>
       </c>
       <c r="K53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>1.0891164594387712</v>
       </c>
       <c r="L53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>1.0381232910441247</v>
       </c>
       <c r="M53" s="4">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>1.0098551278682761</v>
       </c>
       <c r="N53" s="4">
         <f t="shared" ca="1" si="17"/>
@@ -9711,51 +9726,51 @@
       </c>
       <c r="B54" s="4">
         <f ca="1">B53/C53</f>
-        <v>1.8258459273790315</v>
+        <v>2.9207320708831213</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" ref="C54:Y54" ca="1" si="18">C53/D53</f>
-        <v>1.2440255816659809</v>
+        <v>1.8371865633164386</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.1294192410672006</v>
+        <v>1.5128723571281022</v>
       </c>
       <c r="E54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0790691376525661</v>
+        <v>1.3538957236352975</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0502885158504212</v>
+        <v>1.2571792539358313</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0314557926985988</v>
+        <v>1.1909962738973967</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0180698476339016</v>
+        <v>1.1422480792447984</v>
       </c>
       <c r="I54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0080083432212172</v>
+        <v>1.1044912361659469</v>
       </c>
       <c r="J54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1.0001346832030382</v>
+        <v>1.0741628334261819</v>
       </c>
       <c r="K54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>1.0491205320548762</v>
       </c>
       <c r="L54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>1.0279922955241316</v>
       </c>
       <c r="M54" s="4">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>1.0098551278682761</v>
       </c>
       <c r="N54" s="4">
         <f t="shared" ca="1" si="18"/>
@@ -9825,11 +9840,11 @@
       </c>
       <c r="B59" s="4" cm="1">
         <f t="array" aca="1" ref="B59:C59" ca="1">LINEST(LN(IF(B20:P20&lt;=1,1.0001,B20:P20)-1),LN(B2:P2))</f>
-        <v>-4.0921201011967527</v>
+        <v>-4.7032650785067682</v>
       </c>
       <c r="C59" s="4">
         <f ca="1"/>
-        <v>11.889609557632173</v>
+        <v>15.036599693262833</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.35">
@@ -9843,103 +9858,103 @@
       </c>
       <c r="B62" s="4">
         <f ca="1">EXP($C$59+$B$59*LN(B2))+1</f>
-        <v>6.5905244743229829</v>
+        <v>29.486349965572114</v>
       </c>
       <c r="C62" s="4">
         <f t="shared" ref="C62:Z62" ca="1" si="19">EXP($C$59+$B$59*LN(C2))+1</f>
-        <v>1.3277944957769152</v>
+        <v>2.0934852752883728</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0623756487948866</v>
+        <v>1.1624086176775601</v>
       </c>
       <c r="E62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0192198839223674</v>
+        <v>1.0419748422917501</v>
       </c>
       <c r="F62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0077122899381779</v>
+        <v>1.0146958798674344</v>
       </c>
       <c r="G62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0036573302629095</v>
+        <v>1.0062342642081201</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.001946300418612</v>
+        <v>1.0030193725744088</v>
       </c>
       <c r="I62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0011269375866538</v>
+        <v>1.0016112584460295</v>
       </c>
       <c r="J62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0006959492942842</v>
+        <v>1.0009259367777132</v>
       </c>
       <c r="K62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0004522019719584</v>
+        <v>1.0005641202983839</v>
       </c>
       <c r="L62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.000306160115392</v>
+        <v>1.0003603221467747</v>
       </c>
       <c r="M62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0002144436957439</v>
+        <v>1.0002393102704303</v>
       </c>
       <c r="N62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0001545477082883</v>
+        <v>1.0001642350840636</v>
       </c>
       <c r="O62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0001141192686447</v>
+        <v>1.0001159025096131</v>
       </c>
       <c r="P62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000860490086034</v>
+        <v>1.0000837853055133</v>
       </c>
       <c r="Q62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.000066076794706</v>
+        <v>1.0000618502330958</v>
       </c>
       <c r="R62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000515593921184</v>
+        <v>1.0000465060401971</v>
       </c>
       <c r="S62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000408062515518</v>
+        <v>1.0000355432771662</v>
       </c>
       <c r="T62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000327068890822</v>
+        <v>1.0000275625662112</v>
       </c>
       <c r="U62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000265143848432</v>
+        <v>1.0000216544850611</v>
       </c>
       <c r="V62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000217156282776</v>
+        <v>1.000017214284268</v>
       </c>
       <c r="W62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000179513748868</v>
+        <v>1.0000138314302232</v>
       </c>
       <c r="X62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000149657574713</v>
+        <v>1.0000112219887214</v>
       </c>
       <c r="Y62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000125736795253</v>
+        <v>1.0000091862333103</v>
       </c>
       <c r="Z62" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>1.0000106393266612</v>
+        <v>1.0000075814867591</v>
       </c>
     </row>
   </sheetData>
@@ -9952,8 +9967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303009E9-EFA9-49BF-89FB-E97F486B34FD}">
   <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>